<commit_message>
added labels to figures
</commit_message>
<xml_diff>
--- a/eagle/inductor_test/Results.xlsx
+++ b/eagle/inductor_test/Results.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="14385"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="22160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -553,6 +558,25 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>OPA333</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -562,6 +586,9 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Reported</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575">
               <a:noFill/>
@@ -574,58 +601,58 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>30</c:v>
+                  <c:v>30.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>40</c:v>
+                  <c:v>40.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>50</c:v>
+                  <c:v>50.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>75</c:v>
+                  <c:v>75.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>100</c:v>
+                  <c:v>100.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>150</c:v>
+                  <c:v>150.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>200</c:v>
+                  <c:v>200.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>250</c:v>
+                  <c:v>250.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>300</c:v>
+                  <c:v>300.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>350</c:v>
+                  <c:v>350.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>400</c:v>
+                  <c:v>400.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>450</c:v>
+                  <c:v>450.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>500</c:v>
+                  <c:v>500.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -637,58 +664,58 @@
                 <c:formatCode>@</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>1.6669333333333334</c:v>
+                  <c:v>1.666933333333333</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.6638000000000002</c:v>
+                  <c:v>1.6638</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.6575333333333333</c:v>
+                  <c:v>1.657533333333333</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.5854666666666668</c:v>
+                  <c:v>1.585466666666667</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.6575333333333333</c:v>
+                  <c:v>1.657533333333333</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.5384666666666666</c:v>
+                  <c:v>1.538466666666667</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.7703333333333333</c:v>
+                  <c:v>1.770333333333333</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.7170666666666667</c:v>
+                  <c:v>1.717066666666667</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.9708666666666668</c:v>
+                  <c:v>1.970866666666667</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.1933333333333334</c:v>
+                  <c:v>2.193333333333333</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.7009333333333334</c:v>
+                  <c:v>2.700933333333333</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.3401333333333336</c:v>
+                  <c:v>3.340133333333334</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.9323333333333337</c:v>
+                  <c:v>3.932333333333334</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4.6122666666666667</c:v>
+                  <c:v>4.612266666666667</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>5.4614000000000003</c:v>
+                  <c:v>5.4614</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>6.2259333333333338</c:v>
+                  <c:v>6.225933333333334</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>6.981066666666667</c:v>
+                  <c:v>6.981066666666666</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>8.1748666666666665</c:v>
+                  <c:v>8.174866666666666</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -703,8 +730,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="56722944"/>
-        <c:axId val="56721408"/>
+        <c:axId val="-2144913464"/>
+        <c:axId val="-2144910536"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -712,6 +739,9 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:v>Variance</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575">
               <a:noFill/>
@@ -724,58 +754,58 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>30</c:v>
+                  <c:v>30.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>40</c:v>
+                  <c:v>40.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>50</c:v>
+                  <c:v>50.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>75</c:v>
+                  <c:v>75.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>100</c:v>
+                  <c:v>100.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>150</c:v>
+                  <c:v>150.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>200</c:v>
+                  <c:v>200.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>250</c:v>
+                  <c:v>250.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>300</c:v>
+                  <c:v>300.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>350</c:v>
+                  <c:v>350.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>400</c:v>
+                  <c:v>400.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>450</c:v>
+                  <c:v>450.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>500</c:v>
+                  <c:v>500.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -787,58 +817,58 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>5.6844933333333406E-3</c:v>
+                  <c:v>0.00568449333333334</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.4932839999999987E-2</c:v>
+                  <c:v>0.01493284</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.1869693333333341E-2</c:v>
+                  <c:v>0.0118696933333333</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.9733733333333349E-3</c:v>
+                  <c:v>0.00197337333333333</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.9203573333333314E-2</c:v>
+                  <c:v>0.0192035733333333</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.0425293333333353E-2</c:v>
+                  <c:v>0.0304252933333333</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.3648653333333804E-2</c:v>
+                  <c:v>0.0636486533333338</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.1543333333333354E-3</c:v>
+                  <c:v>0.00515433333333333</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.6994573333333363E-2</c:v>
+                  <c:v>0.0169945733333334</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.8496693333333349E-2</c:v>
+                  <c:v>0.0184966933333333</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.973373333333331E-3</c:v>
+                  <c:v>0.00197337333333333</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.1235853333333318E-2</c:v>
+                  <c:v>0.0212358533333333</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.4063373333333346E-2</c:v>
+                  <c:v>0.0240633733333333</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4.2972413333333397E-2</c:v>
+                  <c:v>0.0429724133333334</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>6.3707560000000149E-2</c:v>
+                  <c:v>0.0637075600000001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4.3502573333333287E-2</c:v>
+                  <c:v>0.0435025733333333</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5.8523773333333431E-2</c:v>
+                  <c:v>0.0585237733333334</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.61165737333333314</c:v>
+                  <c:v>0.611657373333333</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -853,26 +883,45 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="75240960"/>
-        <c:axId val="99314688"/>
+        <c:axId val="-2144904136"/>
+        <c:axId val="-2144907432"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="56722944"/>
+        <c:axId val="-2144913464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Power (W)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="56721408"/>
+        <c:crossAx val="-2144910536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="56721408"/>
+        <c:axId val="-2144910536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -883,12 +932,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="56722944"/>
+        <c:crossAx val="-2144913464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="99314688"/>
+        <c:axId val="-2144907432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -898,12 +947,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75240960"/>
+        <c:crossAx val="-2144904136"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="75240960"/>
+        <c:axId val="-2144904136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -913,7 +962,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99314688"/>
+        <c:crossAx val="-2144907432"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
@@ -969,58 +1019,58 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>30</c:v>
+                  <c:v>30.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>40</c:v>
+                  <c:v>40.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>50</c:v>
+                  <c:v>50.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>75</c:v>
+                  <c:v>75.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>100</c:v>
+                  <c:v>100.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>150</c:v>
+                  <c:v>150.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>200</c:v>
+                  <c:v>200.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>250</c:v>
+                  <c:v>250.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>300</c:v>
+                  <c:v>300.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>350</c:v>
+                  <c:v>350.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>400</c:v>
+                  <c:v>400.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>450</c:v>
+                  <c:v>450.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>500</c:v>
+                  <c:v>500.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1038,16 +1088,16 @@
                   <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.20799999999999999</c:v>
+                  <c:v>0.208</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.20799999999999999</c:v>
+                  <c:v>0.208</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.23200000000000001</c:v>
+                  <c:v>0.232</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.27200000000000002</c:v>
+                  <c:v>0.272</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.312</c:v>
@@ -1062,7 +1112,7 @@
                   <c:v>0.78</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.1000000000000001</c:v>
+                  <c:v>1.1</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>1.4</c:v>
@@ -1098,11 +1148,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="73652864"/>
-        <c:axId val="73651328"/>
+        <c:axId val="-2144845736"/>
+        <c:axId val="-2144842776"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="73652864"/>
+        <c:axId val="-2144845736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1112,12 +1162,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73651328"/>
+        <c:crossAx val="-2144842776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="73651328"/>
+        <c:axId val="-2144842776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1128,7 +1178,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73652864"/>
+        <c:crossAx val="-2144845736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1159,6 +1209,25 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>MAX4238</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -1168,6 +1237,9 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Reported</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575">
               <a:noFill/>
@@ -1180,64 +1252,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>30</c:v>
+                  <c:v>30.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>40</c:v>
+                  <c:v>40.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>50</c:v>
+                  <c:v>50.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>75</c:v>
+                  <c:v>75.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>100</c:v>
+                  <c:v>100.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>150</c:v>
+                  <c:v>150.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>200</c:v>
+                  <c:v>200.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>250</c:v>
+                  <c:v>250.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>300</c:v>
+                  <c:v>300.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>350</c:v>
+                  <c:v>350.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>400</c:v>
+                  <c:v>400.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>425</c:v>
+                  <c:v>425.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>450</c:v>
+                  <c:v>450.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>475</c:v>
+                  <c:v>475.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>500</c:v>
+                  <c:v>500.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1249,64 +1321,64 @@
                 <c:formatCode>@</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>1.8674666666666668</c:v>
+                  <c:v>1.867466666666667</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.8768666666666667</c:v>
+                  <c:v>1.876866666666667</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.0993333333333335</c:v>
+                  <c:v>2.099333333333333</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.9614666666666667</c:v>
+                  <c:v>1.961466666666667</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.8894000000000002</c:v>
+                  <c:v>1.8894</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.9458000000000002</c:v>
+                  <c:v>1.9458</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.9677333333333333</c:v>
+                  <c:v>1.967733333333333</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.1776666666666666</c:v>
+                  <c:v>2.177666666666667</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.2184000000000004</c:v>
+                  <c:v>2.2184</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>2.497266666666667</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.9923333333333333</c:v>
+                  <c:v>2.992333333333333</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.6127333333333334</c:v>
+                  <c:v>3.612733333333333</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4.2237333333333336</c:v>
+                  <c:v>4.223733333333333</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4.9694666666666665</c:v>
+                  <c:v>4.969466666666666</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>5.7277333333333331</c:v>
+                  <c:v>5.727733333333333</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>6.4797333333333329</c:v>
+                  <c:v>6.479733333333332</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>6.8870666666666667</c:v>
+                  <c:v>6.887066666666667</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>7.3100666666666667</c:v>
+                  <c:v>7.310066666666667</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>7.8740666666666668</c:v>
+                  <c:v>7.874066666666667</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>10.214666666666666</c:v>
+                  <c:v>10.21466666666667</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1321,8 +1393,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="75421568"/>
-        <c:axId val="75423104"/>
+        <c:axId val="-2144811560"/>
+        <c:axId val="-2144808632"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -1330,6 +1402,9 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:v>Variance</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575">
               <a:noFill/>
@@ -1342,64 +1417,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>30</c:v>
+                  <c:v>30.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>40</c:v>
+                  <c:v>40.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>50</c:v>
+                  <c:v>50.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>75</c:v>
+                  <c:v>75.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>100</c:v>
+                  <c:v>100.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>150</c:v>
+                  <c:v>150.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>200</c:v>
+                  <c:v>200.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>250</c:v>
+                  <c:v>250.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>300</c:v>
+                  <c:v>300.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>350</c:v>
+                  <c:v>350.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>400</c:v>
+                  <c:v>400.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>425</c:v>
+                  <c:v>425.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>450</c:v>
+                  <c:v>450.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>475</c:v>
+                  <c:v>475.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>500</c:v>
+                  <c:v>500.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1411,64 +1486,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>2.945333333333325E-3</c:v>
+                  <c:v>0.00294533333333332</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.9172933333333224E-3</c:v>
+                  <c:v>0.00391729333333332</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.2576573333333375E-2</c:v>
+                  <c:v>0.0125765733333334</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.9776133333333502E-3</c:v>
+                  <c:v>0.00497761333333335</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.9201199999999905E-3</c:v>
+                  <c:v>0.00592011999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.217480000000001E-3</c:v>
+                  <c:v>0.00821748</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.1692973333333327E-2</c:v>
+                  <c:v>0.0116929733333333</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.4432133333333217E-3</c:v>
+                  <c:v>0.00144321333333332</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.3488439999999994E-2</c:v>
+                  <c:v>0.03348844</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.11180485333333223</c:v>
+                  <c:v>0.111804853333332</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9.8462493333333317E-2</c:v>
+                  <c:v>0.0984624933333333</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7.4428573333333303E-2</c:v>
+                  <c:v>0.0744285733333333</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.10111329333333338</c:v>
+                  <c:v>0.101113293333333</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>9.9169373333333463E-2</c:v>
+                  <c:v>0.0991693733333334</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4.0321613333333256E-2</c:v>
+                  <c:v>0.0403216133333332</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>7.5047093333333398E-2</c:v>
+                  <c:v>0.0750470933333334</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>8.5296853333333325E-2</c:v>
+                  <c:v>0.0852968533333333</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.8054893333333249E-2</c:v>
+                  <c:v>0.0180548933333332</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>6.294177333333327E-2</c:v>
+                  <c:v>0.0629417733333333</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.9188253333333452E-2</c:v>
+                  <c:v>0.0291882533333334</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1483,26 +1558,45 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="75389568"/>
-        <c:axId val="75388032"/>
+        <c:axId val="-2144802232"/>
+        <c:axId val="-2144805528"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="75421568"/>
+        <c:axId val="-2144811560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Power (W)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75423104"/>
+        <c:crossAx val="-2144808632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="75423104"/>
+        <c:axId val="-2144808632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1513,12 +1607,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75421568"/>
+        <c:crossAx val="-2144811560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="75388032"/>
+        <c:axId val="-2144805528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1528,12 +1622,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75389568"/>
+        <c:crossAx val="-2144802232"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="75389568"/>
+        <c:axId val="-2144802232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1543,7 +1637,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75388032"/>
+        <c:crossAx val="-2144805528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1600,64 +1694,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>30</c:v>
+                  <c:v>30.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>40</c:v>
+                  <c:v>40.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>50</c:v>
+                  <c:v>50.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>75</c:v>
+                  <c:v>75.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>100</c:v>
+                  <c:v>100.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>150</c:v>
+                  <c:v>150.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>200</c:v>
+                  <c:v>200.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>250</c:v>
+                  <c:v>250.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>300</c:v>
+                  <c:v>300.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>350</c:v>
+                  <c:v>350.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>400</c:v>
+                  <c:v>400.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>425</c:v>
+                  <c:v>425.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>450</c:v>
+                  <c:v>450.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>475</c:v>
+                  <c:v>475.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>500</c:v>
+                  <c:v>500.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1669,19 +1763,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>0.16800000000000001</c:v>
+                  <c:v>0.168</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.16800000000000001</c:v>
+                  <c:v>0.168</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.16800000000000001</c:v>
+                  <c:v>0.168</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.16800000000000001</c:v>
+                  <c:v>0.168</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.20799999999999999</c:v>
+                  <c:v>0.208</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.248</c:v>
@@ -1699,7 +1793,7 @@
                   <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.1399999999999999</c:v>
+                  <c:v>1.14</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>1.56</c:v>
@@ -1708,7 +1802,7 @@
                   <c:v>1.86</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.2400000000000002</c:v>
+                  <c:v>2.24</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>2.64</c:v>
@@ -1741,11 +1835,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="75350016"/>
-        <c:axId val="98900608"/>
+        <c:axId val="-2144781048"/>
+        <c:axId val="-2144778088"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="75350016"/>
+        <c:axId val="-2144781048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1755,12 +1849,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98900608"/>
+        <c:crossAx val="-2144778088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="98900608"/>
+        <c:axId val="-2144778088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1771,7 +1865,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75350016"/>
+        <c:crossAx val="-2144781048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1802,6 +1896,25 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>"Ideal"</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -1811,6 +1924,9 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Reported</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575">
               <a:noFill/>
@@ -1823,58 +1939,58 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>1.5101449275362311</c:v>
+                  <c:v>1.510144927536231</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.9391304347826068</c:v>
+                  <c:v>5.939130434782606</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.368115942028984</c:v>
+                  <c:v>10.36811594202898</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>19.226086956521733</c:v>
+                  <c:v>19.22608695652173</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>28.084057971014488</c:v>
+                  <c:v>28.08405797101449</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>41.371014492753616</c:v>
+                  <c:v>41.37101449275362</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>50.228985507246371</c:v>
+                  <c:v>50.22898550724637</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>67.944927536231873</c:v>
+                  <c:v>67.94492753623187</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>81.231884057970987</c:v>
+                  <c:v>81.23188405797098</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>98.947826086956496</c:v>
+                  <c:v>98.9478260869565</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>152.09565217391301</c:v>
+                  <c:v>152.095652173913</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>200.81449275362317</c:v>
+                  <c:v>200.8144927536232</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>249.5333333333333</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>302.68115942028982</c:v>
+                  <c:v>302.6811594202898</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>351.4</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>400.11884057971014</c:v>
+                  <c:v>400.1188405797101</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>448.83768115942024</c:v>
+                  <c:v>448.8376811594202</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>493.12753623188399</c:v>
+                  <c:v>493.127536231884</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1886,49 +2002,49 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>3.6565999999999996</c:v>
+                  <c:v>3.6566</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.5093333333333327</c:v>
+                  <c:v>3.509333333333333</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.4278666666666666</c:v>
+                  <c:v>3.427866666666667</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.4278666666666666</c:v>
+                  <c:v>3.427866666666667</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.3213333333333335</c:v>
+                  <c:v>3.321333333333333</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.3652000000000002</c:v>
+                  <c:v>3.3652</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.3432666666666666</c:v>
+                  <c:v>3.343266666666667</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.3777333333333335</c:v>
+                  <c:v>3.377733333333333</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.3683333333333336</c:v>
+                  <c:v>3.368333333333334</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.4028000000000005</c:v>
+                  <c:v>3.4028</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.7098666666666666</c:v>
+                  <c:v>3.709866666666667</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.1673333333333336</c:v>
+                  <c:v>4.167333333333334</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4.6279333333333339</c:v>
+                  <c:v>4.627933333333334</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5.2765333333333331</c:v>
+                  <c:v>5.276533333333333</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>5.8373999999999997</c:v>
+                  <c:v>5.8374</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>6.495400000000001</c:v>
@@ -1937,7 +2053,7 @@
                   <c:v>7.150266666666667</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>7.4510666666666667</c:v>
+                  <c:v>7.451066666666666</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1952,8 +2068,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="98886016"/>
-        <c:axId val="98888320"/>
+        <c:axId val="-2144746984"/>
+        <c:axId val="-2144743992"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -1961,6 +2077,9 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:v>Variance</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575">
               <a:noFill/>
@@ -1973,58 +2092,58 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>1.5101449275362311</c:v>
+                  <c:v>1.510144927536231</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.9391304347826068</c:v>
+                  <c:v>5.939130434782606</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.368115942028984</c:v>
+                  <c:v>10.36811594202898</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>19.226086956521733</c:v>
+                  <c:v>19.22608695652173</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>28.084057971014488</c:v>
+                  <c:v>28.08405797101449</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>41.371014492753616</c:v>
+                  <c:v>41.37101449275362</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>50.228985507246371</c:v>
+                  <c:v>50.22898550724637</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>67.944927536231873</c:v>
+                  <c:v>67.94492753623187</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>81.231884057970987</c:v>
+                  <c:v>81.23188405797098</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>98.947826086956496</c:v>
+                  <c:v>98.9478260869565</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>152.09565217391301</c:v>
+                  <c:v>152.095652173913</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>200.81449275362317</c:v>
+                  <c:v>200.8144927536232</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>249.5333333333333</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>302.68115942028982</c:v>
+                  <c:v>302.6811594202898</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>351.4</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>400.11884057971014</c:v>
+                  <c:v>400.1188405797101</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>448.83768115942024</c:v>
+                  <c:v>448.8376811594202</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>493.12753623188399</c:v>
+                  <c:v>493.127536231884</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2036,58 +2155,58 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>2.7656679999999958E-2</c:v>
+                  <c:v>0.02765668</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.5830573333333308E-2</c:v>
+                  <c:v>0.0258305733333333</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.0940133333333233E-3</c:v>
+                  <c:v>0.00409401333333332</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.3310533333333372E-3</c:v>
+                  <c:v>0.00533105333333334</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.6802533333333441E-3</c:v>
+                  <c:v>0.00268025333333334</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.0234440000000034E-2</c:v>
+                  <c:v>0.02023444</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.3782973333333362E-2</c:v>
+                  <c:v>0.0337829733333334</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.1028493333333312E-2</c:v>
+                  <c:v>0.0410284933333333</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.5711573333333269E-2</c:v>
+                  <c:v>0.0457115733333333</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.13050771999999994</c:v>
+                  <c:v>0.13050772</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.11401385333333325</c:v>
+                  <c:v>0.114013853333333</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>9.227729333333333E-2</c:v>
+                  <c:v>0.0922772933333333</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.11790169333333346</c:v>
+                  <c:v>0.117901693333333</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.18885477333333345</c:v>
+                  <c:v>0.188854773333333</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.14959348000000014</c:v>
+                  <c:v>0.14959348</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.12865215999999982</c:v>
+                  <c:v>0.12865216</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.1569568133333335</c:v>
+                  <c:v>0.156956813333333</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.24973481333333339</c:v>
+                  <c:v>0.249734813333333</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2102,26 +2221,45 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="99120640"/>
-        <c:axId val="98898304"/>
+        <c:axId val="-2144737656"/>
+        <c:axId val="-2144740952"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="98886016"/>
+        <c:axId val="-2144746984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Power (W)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98888320"/>
+        <c:crossAx val="-2144743992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="98888320"/>
+        <c:axId val="-2144743992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2132,12 +2270,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98886016"/>
+        <c:crossAx val="-2144746984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="98898304"/>
+        <c:axId val="-2144740952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2147,12 +2285,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99120640"/>
+        <c:crossAx val="-2144737656"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="99120640"/>
+        <c:axId val="-2144737656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2162,7 +2300,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98898304"/>
+        <c:crossAx val="-2144740952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2219,58 +2357,58 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>1.5101449275362311</c:v>
+                  <c:v>1.510144927536231</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.9391304347826068</c:v>
+                  <c:v>5.939130434782606</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.368115942028984</c:v>
+                  <c:v>10.36811594202898</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>19.226086956521733</c:v>
+                  <c:v>19.22608695652173</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>28.084057971014488</c:v>
+                  <c:v>28.08405797101449</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>41.371014492753616</c:v>
+                  <c:v>41.37101449275362</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>50.228985507246371</c:v>
+                  <c:v>50.22898550724637</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>67.944927536231873</c:v>
+                  <c:v>67.94492753623187</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>81.231884057970987</c:v>
+                  <c:v>81.23188405797098</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>98.947826086956496</c:v>
+                  <c:v>98.9478260869565</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>152.09565217391301</c:v>
+                  <c:v>152.095652173913</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>200.81449275362317</c:v>
+                  <c:v>200.8144927536232</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>249.5333333333333</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>302.68115942028982</c:v>
+                  <c:v>302.6811594202898</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>351.4</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>400.11884057971014</c:v>
+                  <c:v>400.1188405797101</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>448.83768115942024</c:v>
+                  <c:v>448.8376811594202</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>493.12753623188399</c:v>
+                  <c:v>493.127536231884</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2282,13 +2420,13 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="28"/>
                 <c:pt idx="0">
-                  <c:v>0.16800000000000001</c:v>
+                  <c:v>0.168</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.184</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.20799999999999999</c:v>
+                  <c:v>0.208</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.24</c:v>
@@ -2297,7 +2435,7 @@
                   <c:v>0.312</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.41599999999999998</c:v>
+                  <c:v>0.416</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.432</c:v>
@@ -2312,7 +2450,7 @@
                   <c:v>0.82</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.1000000000000001</c:v>
+                  <c:v>1.1</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>1.48</c:v>
@@ -2348,11 +2486,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="73894144"/>
-        <c:axId val="73892608"/>
+        <c:axId val="-2144716040"/>
+        <c:axId val="-2144713000"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="73894144"/>
+        <c:axId val="-2144716040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2362,12 +2500,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73892608"/>
+        <c:crossAx val="-2144713000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="73892608"/>
+        <c:axId val="-2144713000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2378,7 +2516,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73894144"/>
+        <c:crossAx val="-2144716040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2880,26 +3018,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K75" sqref="K75:L75"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="U50" sqref="U50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" customWidth="1"/>
-    <col min="3" max="5" width="9.140625" style="2"/>
-    <col min="6" max="6" width="9.140625" style="4" customWidth="1"/>
-    <col min="7" max="8" width="9.140625" style="4" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="1" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" customWidth="1"/>
+    <col min="3" max="5" width="8.83203125" style="2"/>
+    <col min="6" max="6" width="9.1640625" style="4" customWidth="1"/>
+    <col min="7" max="8" width="9.1640625" style="4" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="9.1640625" style="1" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1">
         <v>9.4000000000000004E-3</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2907,7 +3045,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -2925,7 +3063,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11">
       <c r="A4">
         <v>0</v>
       </c>
@@ -2942,15 +3080,15 @@
         <v>7</v>
       </c>
       <c r="G4" s="2">
-        <f>HEX2DEC(C4)*$A$1</f>
+        <f t="shared" ref="G4:G21" si="0">HEX2DEC(C4)*$A$1</f>
         <v>1.6732</v>
       </c>
       <c r="H4" s="2">
-        <f>HEX2DEC(D4)*$A$1</f>
+        <f t="shared" ref="H4:H21" si="1">HEX2DEC(D4)*$A$1</f>
         <v>1.5886</v>
       </c>
       <c r="I4" s="2">
-        <f>HEX2DEC(E4)*$A$1</f>
+        <f t="shared" ref="I4:I21" si="2">HEX2DEC(E4)*$A$1</f>
         <v>1.7390000000000001</v>
       </c>
       <c r="J4" s="2">
@@ -2962,7 +3100,7 @@
         <v>5.6844933333333406E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11">
       <c r="A5">
         <v>2</v>
       </c>
@@ -2979,27 +3117,27 @@
         <v>12</v>
       </c>
       <c r="G5" s="2">
-        <f>HEX2DEC(C5)*$A$1</f>
+        <f t="shared" si="0"/>
         <v>1.7390000000000001</v>
       </c>
       <c r="H5" s="2">
-        <f>HEX2DEC(D5)*$A$1</f>
+        <f t="shared" si="1"/>
         <v>1.5228000000000002</v>
       </c>
       <c r="I5" s="2">
-        <f>HEX2DEC(E5)*$A$1</f>
+        <f t="shared" si="2"/>
         <v>1.7296</v>
       </c>
       <c r="J5" s="2">
-        <f t="shared" ref="J5:J21" si="0">AVERAGE(G5:I5)</f>
+        <f t="shared" ref="J5:J21" si="3">AVERAGE(G5:I5)</f>
         <v>1.6638000000000002</v>
       </c>
       <c r="K5">
-        <f t="shared" ref="K5:K21" si="1">VAR(G5:I5)</f>
+        <f t="shared" ref="K5:K21" si="4">VAR(G5:I5)</f>
         <v>1.4932839999999987E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3016,27 +3154,27 @@
         <v>12</v>
       </c>
       <c r="G6" s="2">
-        <f>HEX2DEC(C6)*$A$1</f>
+        <f t="shared" si="0"/>
         <v>1.7108000000000001</v>
       </c>
       <c r="H6" s="2">
-        <f>HEX2DEC(D6)*$A$1</f>
+        <f t="shared" si="1"/>
         <v>1.5322</v>
       </c>
       <c r="I6" s="2">
-        <f>HEX2DEC(E6)*$A$1</f>
+        <f t="shared" si="2"/>
         <v>1.7296</v>
       </c>
       <c r="J6" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1.6575333333333333</v>
       </c>
       <c r="K6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1.1869693333333341E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11">
       <c r="A7">
         <v>10</v>
       </c>
@@ -3053,27 +3191,27 @@
         <v>21</v>
       </c>
       <c r="G7" s="2">
-        <f>HEX2DEC(C7)*$A$1</f>
+        <f t="shared" si="0"/>
         <v>1.5510000000000002</v>
       </c>
       <c r="H7" s="2">
-        <f>HEX2DEC(D7)*$A$1</f>
+        <f t="shared" si="1"/>
         <v>1.6356000000000002</v>
       </c>
       <c r="I7" s="2">
-        <f>HEX2DEC(E7)*$A$1</f>
+        <f t="shared" si="2"/>
         <v>1.5698000000000001</v>
       </c>
       <c r="J7" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1.5854666666666668</v>
       </c>
       <c r="K7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1.9733733333333349E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11">
       <c r="A8">
         <v>20</v>
       </c>
@@ -3090,27 +3228,27 @@
         <v>19</v>
       </c>
       <c r="G8" s="2">
-        <f>HEX2DEC(C8)*$A$1</f>
+        <f t="shared" si="0"/>
         <v>1.8142</v>
       </c>
       <c r="H8" s="2">
-        <f>HEX2DEC(D8)*$A$1</f>
+        <f t="shared" si="1"/>
         <v>1.6074000000000002</v>
       </c>
       <c r="I8" s="2">
-        <f>HEX2DEC(E8)*$A$1</f>
+        <f t="shared" si="2"/>
         <v>1.5510000000000002</v>
       </c>
       <c r="J8" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1.6575333333333333</v>
       </c>
       <c r="K8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1.9203573333333314E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11">
       <c r="A9">
         <v>30</v>
       </c>
@@ -3127,27 +3265,27 @@
         <v>11</v>
       </c>
       <c r="G9" s="2">
-        <f>HEX2DEC(C9)*$A$1</f>
+        <f t="shared" si="0"/>
         <v>1.3724000000000001</v>
       </c>
       <c r="H9" s="2">
-        <f>HEX2DEC(D9)*$A$1</f>
+        <f t="shared" si="1"/>
         <v>1.7202000000000002</v>
       </c>
       <c r="I9" s="2">
-        <f>HEX2DEC(E9)*$A$1</f>
+        <f t="shared" si="2"/>
         <v>1.5228000000000002</v>
       </c>
       <c r="J9" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1.5384666666666666</v>
       </c>
       <c r="K9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>3.0425293333333353E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11">
       <c r="A10">
         <v>40</v>
       </c>
@@ -3164,27 +3302,27 @@
         <v>31</v>
       </c>
       <c r="G10" s="2">
-        <f>HEX2DEC(C10)*$A$1</f>
+        <f t="shared" si="0"/>
         <v>1.9646000000000001</v>
       </c>
       <c r="H10" s="2">
-        <f>HEX2DEC(D10)*$A$1</f>
+        <f t="shared" si="1"/>
         <v>1.8612</v>
       </c>
       <c r="I10" s="2">
-        <f>HEX2DEC(E10)*$A$1</f>
+        <f t="shared" si="2"/>
         <v>1.4852000000000001</v>
       </c>
       <c r="J10" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1.7703333333333333</v>
       </c>
       <c r="K10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>6.3648653333333804E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11">
       <c r="A11">
         <v>50</v>
       </c>
@@ -3201,27 +3339,27 @@
         <v>34</v>
       </c>
       <c r="G11" s="2">
-        <f>HEX2DEC(C11)*$A$1</f>
+        <f t="shared" si="0"/>
         <v>1.6544000000000001</v>
       </c>
       <c r="H11" s="2">
-        <f>HEX2DEC(D11)*$A$1</f>
+        <f t="shared" si="1"/>
         <v>1.7954000000000001</v>
       </c>
       <c r="I11" s="2">
-        <f>HEX2DEC(E11)*$A$1</f>
+        <f t="shared" si="2"/>
         <v>1.7014</v>
       </c>
       <c r="J11" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1.7170666666666667</v>
       </c>
       <c r="K11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>5.1543333333333354E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11">
       <c r="A12">
         <v>75</v>
       </c>
@@ -3238,27 +3376,27 @@
         <v>30</v>
       </c>
       <c r="G12" s="2">
-        <f>HEX2DEC(C12)*$A$1</f>
+        <f t="shared" si="0"/>
         <v>2.1150000000000002</v>
       </c>
       <c r="H12" s="2">
-        <f>HEX2DEC(D12)*$A$1</f>
+        <f t="shared" si="1"/>
         <v>1.9364000000000001</v>
       </c>
       <c r="I12" s="2">
-        <f>HEX2DEC(E12)*$A$1</f>
+        <f t="shared" si="2"/>
         <v>1.8612</v>
       </c>
       <c r="J12" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1.9708666666666668</v>
       </c>
       <c r="K12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1.6994573333333363E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11">
       <c r="A13">
         <v>100</v>
       </c>
@@ -3275,27 +3413,27 @@
         <v>10</v>
       </c>
       <c r="G13" s="2">
-        <f>HEX2DEC(C13)*$A$1</f>
+        <f t="shared" si="0"/>
         <v>2.1055999999999999</v>
       </c>
       <c r="H13" s="2">
-        <f>HEX2DEC(D13)*$A$1</f>
+        <f t="shared" si="1"/>
         <v>2.1244000000000001</v>
       </c>
       <c r="I13" s="2">
-        <f>HEX2DEC(E13)*$A$1</f>
+        <f t="shared" si="2"/>
         <v>2.35</v>
       </c>
       <c r="J13" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>2.1933333333333334</v>
       </c>
       <c r="K13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1.8496693333333349E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11">
       <c r="A14">
         <v>150</v>
       </c>
@@ -3312,27 +3450,27 @@
         <v>39</v>
       </c>
       <c r="G14" s="2">
-        <f>HEX2DEC(C14)*$A$1</f>
+        <f t="shared" si="0"/>
         <v>2.6508000000000003</v>
       </c>
       <c r="H14" s="2">
-        <f>HEX2DEC(D14)*$A$1</f>
+        <f t="shared" si="1"/>
         <v>2.7354000000000003</v>
       </c>
       <c r="I14" s="2">
-        <f>HEX2DEC(E14)*$A$1</f>
+        <f t="shared" si="2"/>
         <v>2.7166000000000001</v>
       </c>
       <c r="J14" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>2.7009333333333334</v>
       </c>
       <c r="K14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1.973373333333331E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11">
       <c r="A15">
         <v>200</v>
       </c>
@@ -3349,27 +3487,27 @@
         <v>42</v>
       </c>
       <c r="G15" s="2">
-        <f>HEX2DEC(C15)*$A$1</f>
+        <f t="shared" si="0"/>
         <v>3.1960000000000002</v>
       </c>
       <c r="H15" s="2">
-        <f>HEX2DEC(D15)*$A$1</f>
+        <f t="shared" si="1"/>
         <v>3.3370000000000002</v>
       </c>
       <c r="I15" s="2">
-        <f>HEX2DEC(E15)*$A$1</f>
+        <f t="shared" si="2"/>
         <v>3.4874000000000001</v>
       </c>
       <c r="J15" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>3.3401333333333336</v>
       </c>
       <c r="K15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>2.1235853333333318E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11">
       <c r="A16">
         <v>250</v>
       </c>
@@ -3386,27 +3524,27 @@
         <v>45</v>
       </c>
       <c r="G16" s="2">
-        <f>HEX2DEC(C16)*$A$1</f>
+        <f t="shared" si="0"/>
         <v>3.9762</v>
       </c>
       <c r="H16" s="2">
-        <f>HEX2DEC(D16)*$A$1</f>
+        <f t="shared" si="1"/>
         <v>3.7600000000000002</v>
       </c>
       <c r="I16" s="2">
-        <f>HEX2DEC(E16)*$A$1</f>
+        <f t="shared" si="2"/>
         <v>4.0608000000000004</v>
       </c>
       <c r="J16" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>3.9323333333333337</v>
       </c>
       <c r="K16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>2.4063373333333346E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11">
       <c r="A17">
         <v>300</v>
       </c>
@@ -3423,27 +3561,27 @@
         <v>48</v>
       </c>
       <c r="G17" s="2">
-        <f>HEX2DEC(C17)*$A$1</f>
+        <f t="shared" si="0"/>
         <v>4.4367999999999999</v>
       </c>
       <c r="H17" s="2">
-        <f>HEX2DEC(D17)*$A$1</f>
+        <f t="shared" si="1"/>
         <v>4.8410000000000002</v>
       </c>
       <c r="I17" s="2">
-        <f>HEX2DEC(E17)*$A$1</f>
+        <f t="shared" si="2"/>
         <v>4.5590000000000002</v>
       </c>
       <c r="J17" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>4.6122666666666667</v>
       </c>
       <c r="K17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>4.2972413333333397E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11">
       <c r="A18">
         <v>350</v>
       </c>
@@ -3460,27 +3598,27 @@
         <v>51</v>
       </c>
       <c r="G18" s="2">
-        <f>HEX2DEC(C18)*$A$1</f>
+        <f t="shared" si="0"/>
         <v>5.6118000000000006</v>
       </c>
       <c r="H18" s="2">
-        <f>HEX2DEC(D18)*$A$1</f>
+        <f t="shared" si="1"/>
         <v>5.17</v>
       </c>
       <c r="I18" s="2">
-        <f>HEX2DEC(E18)*$A$1</f>
+        <f t="shared" si="2"/>
         <v>5.6024000000000003</v>
       </c>
       <c r="J18" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>5.4614000000000003</v>
       </c>
       <c r="K18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>6.3707560000000149E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11">
       <c r="A19">
         <v>400</v>
       </c>
@@ -3497,27 +3635,27 @@
         <v>54</v>
       </c>
       <c r="G19" s="2">
-        <f>HEX2DEC(C19)*$A$1</f>
+        <f t="shared" si="0"/>
         <v>6.0348000000000006</v>
       </c>
       <c r="H19" s="2">
-        <f>HEX2DEC(D19)*$A$1</f>
+        <f t="shared" si="1"/>
         <v>6.4484000000000004</v>
       </c>
       <c r="I19" s="2">
-        <f>HEX2DEC(E19)*$A$1</f>
+        <f t="shared" si="2"/>
         <v>6.1946000000000003</v>
       </c>
       <c r="J19" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>6.2259333333333338</v>
       </c>
       <c r="K19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>4.3502573333333287E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11">
       <c r="A20">
         <v>450</v>
       </c>
@@ -3534,27 +3672,27 @@
         <v>57</v>
       </c>
       <c r="G20" s="2">
-        <f>HEX2DEC(C20)*$A$1</f>
+        <f t="shared" si="0"/>
         <v>7.1346000000000007</v>
       </c>
       <c r="H20" s="2">
-        <f>HEX2DEC(D20)*$A$1</f>
+        <f t="shared" si="1"/>
         <v>7.1064000000000007</v>
       </c>
       <c r="I20" s="2">
-        <f>HEX2DEC(E20)*$A$1</f>
+        <f t="shared" si="2"/>
         <v>6.7022000000000004</v>
       </c>
       <c r="J20" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>6.981066666666667</v>
       </c>
       <c r="K20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>5.8523773333333431E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11">
       <c r="A21">
         <v>500</v>
       </c>
@@ -3571,39 +3709,39 @@
         <v>15</v>
       </c>
       <c r="G21" s="2">
-        <f>HEX2DEC(C21)*$A$1</f>
+        <f t="shared" si="0"/>
         <v>7.4260000000000002</v>
       </c>
       <c r="H21" s="2">
-        <f>HEX2DEC(D21)*$A$1</f>
+        <f t="shared" si="1"/>
         <v>8.9863999999999997</v>
       </c>
       <c r="I21" s="2">
-        <f>HEX2DEC(E21)*$A$1</f>
+        <f t="shared" si="2"/>
         <v>8.1121999999999996</v>
       </c>
       <c r="J21" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>8.1748666666666665</v>
       </c>
       <c r="K21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.61165737333333314</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11">
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11">
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11">
       <c r="A24" t="s">
         <v>59</v>
       </c>
@@ -3615,7 +3753,7 @@
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11">
       <c r="A25" t="s">
         <v>1</v>
       </c>
@@ -3635,7 +3773,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11">
       <c r="A26">
         <v>0</v>
       </c>
@@ -3652,27 +3790,27 @@
         <v>60</v>
       </c>
       <c r="G26" s="2">
-        <f>HEX2DEC(C26)*$A$1</f>
+        <f t="shared" ref="G26:G45" si="5">HEX2DEC(C26)*$A$1</f>
         <v>1.8988</v>
       </c>
       <c r="H26" s="2">
-        <f>HEX2DEC(D26)*$A$1</f>
+        <f t="shared" ref="H26:H45" si="6">HEX2DEC(D26)*$A$1</f>
         <v>1.8048000000000002</v>
       </c>
       <c r="I26" s="2">
-        <f>HEX2DEC(E26)*$A$1</f>
+        <f t="shared" ref="I26:I45" si="7">HEX2DEC(E26)*$A$1</f>
         <v>1.8988</v>
       </c>
       <c r="J26" s="2">
-        <f t="shared" ref="J26:J45" si="2">AVERAGE(G26:I26)</f>
+        <f t="shared" ref="J26:J45" si="8">AVERAGE(G26:I26)</f>
         <v>1.8674666666666668</v>
       </c>
       <c r="K26">
-        <f t="shared" ref="K26:K45" si="3">VAR(G26:I26)</f>
+        <f t="shared" ref="K26:K45" si="9">VAR(G26:I26)</f>
         <v>2.945333333333325E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11">
       <c r="A27">
         <v>2</v>
       </c>
@@ -3689,27 +3827,27 @@
         <v>63</v>
       </c>
       <c r="G27" s="2">
-        <f>HEX2DEC(C27)*$A$1</f>
+        <f t="shared" si="5"/>
         <v>1.8048000000000002</v>
       </c>
       <c r="H27" s="2">
-        <f>HEX2DEC(D27)*$A$1</f>
+        <f t="shared" si="6"/>
         <v>1.9176</v>
       </c>
       <c r="I27" s="2">
-        <f>HEX2DEC(E27)*$A$1</f>
+        <f t="shared" si="7"/>
         <v>1.9082000000000001</v>
       </c>
       <c r="J27" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>1.8768666666666667</v>
       </c>
       <c r="K27">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>3.9172933333333224E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11">
       <c r="A28">
         <v>5</v>
       </c>
@@ -3726,27 +3864,27 @@
         <v>69</v>
       </c>
       <c r="G28" s="2">
-        <f>HEX2DEC(C28)*$A$1</f>
+        <f t="shared" si="5"/>
         <v>2.2278000000000002</v>
       </c>
       <c r="H28" s="2">
-        <f>HEX2DEC(D28)*$A$1</f>
+        <f t="shared" si="6"/>
         <v>2.0209999999999999</v>
       </c>
       <c r="I28" s="2">
-        <f>HEX2DEC(E28)*$A$1</f>
+        <f t="shared" si="7"/>
         <v>2.0491999999999999</v>
       </c>
       <c r="J28" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>2.0993333333333335</v>
       </c>
       <c r="K28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1.2576573333333375E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11">
       <c r="A29">
         <v>10</v>
       </c>
@@ -3763,27 +3901,27 @@
         <v>71</v>
       </c>
       <c r="G29" s="2">
-        <f>HEX2DEC(C29)*$A$1</f>
+        <f t="shared" si="5"/>
         <v>1.9646000000000001</v>
       </c>
       <c r="H29" s="2">
-        <f>HEX2DEC(D29)*$A$1</f>
+        <f t="shared" si="6"/>
         <v>1.8894</v>
       </c>
       <c r="I29" s="2">
-        <f>HEX2DEC(E29)*$A$1</f>
+        <f t="shared" si="7"/>
         <v>2.0304000000000002</v>
       </c>
       <c r="J29" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>1.9614666666666667</v>
       </c>
       <c r="K29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>4.9776133333333502E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11">
       <c r="A30">
         <v>20</v>
       </c>
@@ -3800,27 +3938,27 @@
         <v>72</v>
       </c>
       <c r="G30" s="2">
-        <f>HEX2DEC(C30)*$A$1</f>
+        <f t="shared" si="5"/>
         <v>1.9082000000000001</v>
       </c>
       <c r="H30" s="2">
-        <f>HEX2DEC(D30)*$A$1</f>
+        <f t="shared" si="6"/>
         <v>1.8048000000000002</v>
       </c>
       <c r="I30" s="2">
-        <f>HEX2DEC(E30)*$A$1</f>
+        <f t="shared" si="7"/>
         <v>1.9552</v>
       </c>
       <c r="J30" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>1.8894000000000002</v>
       </c>
       <c r="K30">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>5.9201199999999905E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3837,27 +3975,27 @@
         <v>75</v>
       </c>
       <c r="G31" s="2">
-        <f>HEX2DEC(C31)*$A$1</f>
+        <f t="shared" si="5"/>
         <v>2.0116000000000001</v>
       </c>
       <c r="H31" s="2">
-        <f>HEX2DEC(D31)*$A$1</f>
+        <f t="shared" si="6"/>
         <v>1.8424</v>
       </c>
       <c r="I31" s="2">
-        <f>HEX2DEC(E31)*$A$1</f>
+        <f t="shared" si="7"/>
         <v>1.9834000000000001</v>
       </c>
       <c r="J31" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>1.9458000000000002</v>
       </c>
       <c r="K31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>8.217480000000001E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11">
       <c r="A32">
         <v>40</v>
       </c>
@@ -3874,27 +4012,27 @@
         <v>29</v>
       </c>
       <c r="G32" s="2">
-        <f>HEX2DEC(C32)*$A$1</f>
+        <f t="shared" si="5"/>
         <v>1.8612</v>
       </c>
       <c r="H32" s="2">
-        <f>HEX2DEC(D32)*$A$1</f>
+        <f t="shared" si="6"/>
         <v>2.0773999999999999</v>
       </c>
       <c r="I32" s="2">
-        <f>HEX2DEC(E32)*$A$1</f>
+        <f t="shared" si="7"/>
         <v>1.9646000000000001</v>
       </c>
       <c r="J32" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>1.9677333333333333</v>
       </c>
       <c r="K32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1.1692973333333327E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11">
       <c r="A33">
         <v>50</v>
       </c>
@@ -3911,27 +4049,27 @@
         <v>79</v>
       </c>
       <c r="G33" s="2">
-        <f>HEX2DEC(C33)*$A$1</f>
+        <f t="shared" si="5"/>
         <v>2.2183999999999999</v>
       </c>
       <c r="H33" s="2">
-        <f>HEX2DEC(D33)*$A$1</f>
+        <f t="shared" si="6"/>
         <v>2.1432000000000002</v>
       </c>
       <c r="I33" s="2">
-        <f>HEX2DEC(E33)*$A$1</f>
+        <f t="shared" si="7"/>
         <v>2.1714000000000002</v>
       </c>
       <c r="J33" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>2.1776666666666666</v>
       </c>
       <c r="K33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>1.4432133333333217E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11">
       <c r="A34">
         <v>75</v>
       </c>
@@ -3948,27 +4086,27 @@
         <v>81</v>
       </c>
       <c r="G34" s="2">
-        <f>HEX2DEC(C34)*$A$1</f>
+        <f t="shared" si="5"/>
         <v>2.0116000000000001</v>
       </c>
       <c r="H34" s="2">
-        <f>HEX2DEC(D34)*$A$1</f>
+        <f t="shared" si="6"/>
         <v>2.3593999999999999</v>
       </c>
       <c r="I34" s="2">
-        <f>HEX2DEC(E34)*$A$1</f>
+        <f t="shared" si="7"/>
         <v>2.2842000000000002</v>
       </c>
       <c r="J34" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>2.2184000000000004</v>
       </c>
       <c r="K34">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>3.3488439999999994E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11">
       <c r="A35">
         <v>100</v>
       </c>
@@ -3985,27 +4123,27 @@
         <v>84</v>
       </c>
       <c r="G35" s="2">
-        <f>HEX2DEC(C35)*$A$1</f>
+        <f t="shared" si="5"/>
         <v>2.7918000000000003</v>
       </c>
       <c r="H35" s="2">
-        <f>HEX2DEC(D35)*$A$1</f>
+        <f t="shared" si="6"/>
         <v>2.1337999999999999</v>
       </c>
       <c r="I35" s="2">
-        <f>HEX2DEC(E35)*$A$1</f>
+        <f t="shared" si="7"/>
         <v>2.5662000000000003</v>
       </c>
       <c r="J35" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>2.497266666666667</v>
       </c>
       <c r="K35">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.11180485333333223</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11">
       <c r="A36">
         <v>150</v>
       </c>
@@ -4022,27 +4160,27 @@
         <v>87</v>
       </c>
       <c r="G36" s="2">
-        <f>HEX2DEC(C36)*$A$1</f>
+        <f t="shared" si="5"/>
         <v>3.2054</v>
       </c>
       <c r="H36" s="2">
-        <f>HEX2DEC(D36)*$A$1</f>
+        <f t="shared" si="6"/>
         <v>2.6320000000000001</v>
       </c>
       <c r="I36" s="2">
-        <f>HEX2DEC(E36)*$A$1</f>
+        <f t="shared" si="7"/>
         <v>3.1396000000000002</v>
       </c>
       <c r="J36" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>2.9923333333333333</v>
       </c>
       <c r="K36">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>9.8462493333333317E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11">
       <c r="A37">
         <v>200</v>
       </c>
@@ -4059,27 +4197,27 @@
         <v>90</v>
       </c>
       <c r="G37" s="2">
-        <f>HEX2DEC(C37)*$A$1</f>
+        <f t="shared" si="5"/>
         <v>3.6002000000000001</v>
       </c>
       <c r="H37" s="2">
-        <f>HEX2DEC(D37)*$A$1</f>
+        <f t="shared" si="6"/>
         <v>3.8915999999999999</v>
       </c>
       <c r="I37" s="2">
-        <f>HEX2DEC(E37)*$A$1</f>
+        <f t="shared" si="7"/>
         <v>3.3464</v>
       </c>
       <c r="J37" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>3.6127333333333334</v>
       </c>
       <c r="K37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>7.4428573333333303E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11">
       <c r="A38">
         <v>250</v>
       </c>
@@ -4096,27 +4234,27 @@
         <v>93</v>
       </c>
       <c r="G38" s="2">
-        <f>HEX2DEC(C38)*$A$1</f>
+        <f t="shared" si="5"/>
         <v>4.4649999999999999</v>
       </c>
       <c r="H38" s="2">
-        <f>HEX2DEC(D38)*$A$1</f>
+        <f t="shared" si="6"/>
         <v>4.3428000000000004</v>
       </c>
       <c r="I38" s="2">
-        <f>HEX2DEC(E38)*$A$1</f>
+        <f t="shared" si="7"/>
         <v>3.8633999999999999</v>
       </c>
       <c r="J38" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>4.2237333333333336</v>
       </c>
       <c r="K38">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0.10111329333333338</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11">
       <c r="A39">
         <v>300</v>
       </c>
@@ -4133,27 +4271,27 @@
         <v>96</v>
       </c>
       <c r="G39" s="2">
-        <f>HEX2DEC(C39)*$A$1</f>
+        <f t="shared" si="5"/>
         <v>5.1606000000000005</v>
       </c>
       <c r="H39" s="2">
-        <f>HEX2DEC(D39)*$A$1</f>
+        <f t="shared" si="6"/>
         <v>4.6059999999999999</v>
       </c>
       <c r="I39" s="2">
-        <f>HEX2DEC(E39)*$A$1</f>
+        <f t="shared" si="7"/>
         <v>5.1417999999999999</v>
       </c>
       <c r="J39" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>4.9694666666666665</v>
       </c>
       <c r="K39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>9.9169373333333463E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11">
       <c r="A40">
         <v>350</v>
       </c>
@@ -4170,27 +4308,27 @@
         <v>99</v>
       </c>
       <c r="G40" s="2">
-        <f>HEX2DEC(C40)*$A$1</f>
+        <f t="shared" si="5"/>
         <v>5.8092000000000006</v>
       </c>
       <c r="H40" s="2">
-        <f>HEX2DEC(D40)*$A$1</f>
+        <f t="shared" si="6"/>
         <v>5.4990000000000006</v>
       </c>
       <c r="I40" s="2">
-        <f>HEX2DEC(E40)*$A$1</f>
+        <f t="shared" si="7"/>
         <v>5.875</v>
       </c>
       <c r="J40" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>5.7277333333333331</v>
       </c>
       <c r="K40">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>4.0321613333333256E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11">
       <c r="A41">
         <v>400</v>
       </c>
@@ -4207,27 +4345,27 @@
         <v>102</v>
       </c>
       <c r="G41" s="2">
-        <f>HEX2DEC(C41)*$A$1</f>
+        <f t="shared" si="5"/>
         <v>6.1664000000000003</v>
       </c>
       <c r="H41" s="2">
-        <f>HEX2DEC(D41)*$A$1</f>
+        <f t="shared" si="6"/>
         <v>6.6740000000000004</v>
       </c>
       <c r="I41" s="2">
-        <f>HEX2DEC(E41)*$A$1</f>
+        <f t="shared" si="7"/>
         <v>6.5988000000000007</v>
       </c>
       <c r="J41" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>6.4797333333333329</v>
       </c>
       <c r="K41">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>7.5047093333333398E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11">
       <c r="A42">
         <v>425</v>
       </c>
@@ -4244,27 +4382,27 @@
         <v>105</v>
       </c>
       <c r="G42" s="2">
-        <f>HEX2DEC(C42)*$A$1</f>
+        <f t="shared" si="5"/>
         <v>6.5612000000000004</v>
       </c>
       <c r="H42" s="2">
-        <f>HEX2DEC(D42)*$A$1</f>
+        <f t="shared" si="6"/>
         <v>6.9748000000000001</v>
       </c>
       <c r="I42" s="2">
-        <f>HEX2DEC(E42)*$A$1</f>
+        <f t="shared" si="7"/>
         <v>7.1252000000000004</v>
       </c>
       <c r="J42" s="2">
-        <f t="shared" ref="J42:J44" si="4">AVERAGE(G42:I42)</f>
+        <f t="shared" ref="J42:J44" si="10">AVERAGE(G42:I42)</f>
         <v>6.8870666666666667</v>
       </c>
       <c r="K42">
-        <f t="shared" ref="K42:K44" si="5">VAR(G42:I42)</f>
+        <f t="shared" ref="K42:K44" si="11">VAR(G42:I42)</f>
         <v>8.5296853333333325E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11">
       <c r="A43">
         <v>450</v>
       </c>
@@ -4281,27 +4419,27 @@
         <v>13</v>
       </c>
       <c r="G43" s="2">
-        <f>HEX2DEC(C43)*$A$1</f>
+        <f t="shared" si="5"/>
         <v>7.1628000000000007</v>
       </c>
       <c r="H43" s="2">
-        <f>HEX2DEC(D43)*$A$1</f>
+        <f t="shared" si="6"/>
         <v>7.3414000000000001</v>
       </c>
       <c r="I43" s="2">
-        <f>HEX2DEC(E43)*$A$1</f>
+        <f t="shared" si="7"/>
         <v>7.4260000000000002</v>
       </c>
       <c r="J43" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>7.3100666666666667</v>
       </c>
       <c r="K43">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>1.8054893333333249E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11">
       <c r="A44">
         <v>475</v>
       </c>
@@ -4318,27 +4456,27 @@
         <v>110</v>
       </c>
       <c r="G44" s="2">
-        <f>HEX2DEC(C44)*$A$1</f>
+        <f t="shared" si="5"/>
         <v>7.8395999999999999</v>
       </c>
       <c r="H44" s="2">
-        <f>HEX2DEC(D44)*$A$1</f>
+        <f t="shared" si="6"/>
         <v>8.1403999999999996</v>
       </c>
       <c r="I44" s="2">
-        <f>HEX2DEC(E44)*$A$1</f>
+        <f t="shared" si="7"/>
         <v>7.6421999999999999</v>
       </c>
       <c r="J44" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="10"/>
         <v>7.8740666666666668</v>
       </c>
       <c r="K44">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>6.294177333333327E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11">
       <c r="A45">
         <v>500</v>
       </c>
@@ -4355,39 +4493,39 @@
         <v>66</v>
       </c>
       <c r="G45" s="2">
-        <f>HEX2DEC(C45)*$A$1</f>
+        <f t="shared" si="5"/>
         <v>10.405800000000001</v>
       </c>
       <c r="H45" s="2">
-        <f>HEX2DEC(D45)*$A$1</f>
+        <f t="shared" si="6"/>
         <v>10.1614</v>
       </c>
       <c r="I45" s="2">
-        <f>HEX2DEC(E45)*$A$1</f>
+        <f t="shared" si="7"/>
         <v>10.0768</v>
       </c>
       <c r="J45" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>10.214666666666666</v>
       </c>
       <c r="K45">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>2.9188253333333452E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11">
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
       <c r="I46" s="2"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11">
       <c r="F47" s="2"/>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
       <c r="I47" s="2"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11">
       <c r="A48" t="s">
         <v>111</v>
       </c>
@@ -4399,7 +4537,7 @@
       <c r="H48" s="2"/>
       <c r="I48" s="2"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12">
       <c r="A49" t="s">
         <v>113</v>
       </c>
@@ -4417,7 +4555,7 @@
       <c r="H49" s="2"/>
       <c r="I49" s="2"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12">
       <c r="A50">
         <v>2</v>
       </c>
@@ -4442,31 +4580,31 @@
         <v>3.6284000000000001</v>
       </c>
       <c r="H50" s="2">
-        <f t="shared" ref="H50:I50" si="6">HEX2DEC(E50)*$A$1</f>
+        <f t="shared" ref="H50:I50" si="12">HEX2DEC(E50)*$A$1</f>
         <v>3.8351999999999999</v>
       </c>
       <c r="I50" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="12"/>
         <v>3.5062000000000002</v>
       </c>
       <c r="J50" s="4">
-        <f>AVERAGE(G50:I50)</f>
+        <f t="shared" ref="J50:J57" si="13">AVERAGE(G50:I50)</f>
         <v>3.6565999999999996</v>
       </c>
       <c r="K50" s="5">
-        <f>VAR(G50:I50)</f>
+        <f t="shared" ref="K50:K57" si="14">VAR(G50:I50)</f>
         <v>2.7656679999999958E-2</v>
       </c>
       <c r="L50" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12">
       <c r="A51">
         <v>3</v>
       </c>
       <c r="B51">
-        <f t="shared" ref="B51:B67" si="7">(A51*30.56-50.7)/6.9</f>
+        <f t="shared" ref="B51:B67" si="15">(A51*30.56-50.7)/6.9</f>
         <v>5.9391304347826068</v>
       </c>
       <c r="C51" s="6">
@@ -4482,32 +4620,32 @@
         <v>116</v>
       </c>
       <c r="G51" s="2">
-        <f t="shared" ref="G51:G66" si="8">HEX2DEC(D51)*$A$1</f>
+        <f t="shared" ref="G51:G56" si="16">HEX2DEC(D51)*$A$1</f>
         <v>3.6941999999999999</v>
       </c>
       <c r="H51" s="2">
-        <f t="shared" ref="H51:H66" si="9">HEX2DEC(E51)*$A$1</f>
+        <f t="shared" ref="H51:H56" si="17">HEX2DEC(E51)*$A$1</f>
         <v>3.431</v>
       </c>
       <c r="I51" s="2">
-        <f t="shared" ref="I51:I66" si="10">HEX2DEC(F51)*$A$1</f>
+        <f t="shared" ref="I51:I56" si="18">HEX2DEC(F51)*$A$1</f>
         <v>3.4028</v>
       </c>
       <c r="J51" s="4">
-        <f>AVERAGE(G51:I51)</f>
+        <f t="shared" si="13"/>
         <v>3.5093333333333327</v>
       </c>
       <c r="K51" s="5">
-        <f>VAR(G51:I51)</f>
+        <f t="shared" si="14"/>
         <v>2.5830573333333308E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12">
       <c r="A52">
         <v>4</v>
       </c>
       <c r="B52">
-        <f t="shared" si="7"/>
+        <f t="shared" si="15"/>
         <v>10.368115942028984</v>
       </c>
       <c r="C52" s="6">
@@ -4523,32 +4661,32 @@
         <v>125</v>
       </c>
       <c r="G52" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="16"/>
         <v>3.4498000000000002</v>
       </c>
       <c r="H52" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>3.4780000000000002</v>
       </c>
       <c r="I52" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>3.3558000000000003</v>
       </c>
       <c r="J52" s="4">
-        <f>AVERAGE(G52:I52)</f>
+        <f t="shared" si="13"/>
         <v>3.4278666666666666</v>
       </c>
       <c r="K52" s="5">
-        <f>VAR(G52:I52)</f>
+        <f t="shared" si="14"/>
         <v>4.0940133333333233E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12">
       <c r="A53">
         <v>6</v>
       </c>
       <c r="B53">
-        <f t="shared" si="7"/>
+        <f t="shared" si="15"/>
         <v>19.226086956521733</v>
       </c>
       <c r="C53" s="6">
@@ -4564,32 +4702,32 @@
         <v>90</v>
       </c>
       <c r="G53" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="16"/>
         <v>3.4874000000000001</v>
       </c>
       <c r="H53" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>3.4498000000000002</v>
       </c>
       <c r="I53" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>3.3464</v>
       </c>
       <c r="J53" s="4">
-        <f>AVERAGE(G53:I53)</f>
+        <f t="shared" si="13"/>
         <v>3.4278666666666666</v>
       </c>
       <c r="K53" s="5">
-        <f>VAR(G53:I53)</f>
+        <f t="shared" si="14"/>
         <v>5.3310533333333372E-3</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12">
       <c r="A54">
         <v>8</v>
       </c>
       <c r="B54">
-        <f t="shared" si="7"/>
+        <f t="shared" si="15"/>
         <v>28.084057971014488</v>
       </c>
       <c r="C54" s="6">
@@ -4605,32 +4743,32 @@
         <v>126</v>
       </c>
       <c r="G54" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="16"/>
         <v>3.3558000000000003</v>
       </c>
       <c r="H54" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>3.3464</v>
       </c>
       <c r="I54" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>3.2618</v>
       </c>
       <c r="J54" s="4">
-        <f>AVERAGE(G54:I54)</f>
+        <f t="shared" si="13"/>
         <v>3.3213333333333335</v>
       </c>
       <c r="K54" s="5">
-        <f>VAR(G54:I54)</f>
+        <f t="shared" si="14"/>
         <v>2.6802533333333441E-3</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12">
       <c r="A55">
         <v>11</v>
       </c>
       <c r="B55">
-        <f t="shared" si="7"/>
+        <f t="shared" si="15"/>
         <v>41.371014492753616</v>
       </c>
       <c r="C55" s="6">
@@ -4646,32 +4784,32 @@
         <v>124</v>
       </c>
       <c r="G55" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="16"/>
         <v>3.2054</v>
       </c>
       <c r="H55" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>3.4122000000000003</v>
       </c>
       <c r="I55" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>3.4780000000000002</v>
       </c>
       <c r="J55" s="4">
-        <f>AVERAGE(G55:I55)</f>
+        <f t="shared" si="13"/>
         <v>3.3652000000000002</v>
       </c>
       <c r="K55" s="5">
-        <f>VAR(G55:I55)</f>
+        <f t="shared" si="14"/>
         <v>2.0234440000000034E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12">
       <c r="A56">
         <v>13</v>
       </c>
       <c r="B56">
-        <f t="shared" si="7"/>
+        <f t="shared" si="15"/>
         <v>50.228985507246371</v>
       </c>
       <c r="C56" s="6">
@@ -4687,32 +4825,32 @@
         <v>128</v>
       </c>
       <c r="G56" s="2">
-        <f t="shared" si="8"/>
+        <f t="shared" si="16"/>
         <v>3.4968000000000004</v>
       </c>
       <c r="H56" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>3.1396000000000002</v>
       </c>
       <c r="I56" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>3.3934000000000002</v>
       </c>
       <c r="J56" s="4">
-        <f>AVERAGE(G56:I56)</f>
+        <f t="shared" si="13"/>
         <v>3.3432666666666666</v>
       </c>
       <c r="K56" s="5">
-        <f>VAR(G56:I56)</f>
+        <f t="shared" si="14"/>
         <v>3.3782973333333362E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12">
       <c r="A57">
         <v>17</v>
       </c>
       <c r="B57">
-        <f t="shared" si="7"/>
+        <f t="shared" si="15"/>
         <v>67.944927536231873</v>
       </c>
       <c r="C57" s="6">
@@ -4728,32 +4866,32 @@
         <v>130</v>
       </c>
       <c r="G57" s="2">
-        <f t="shared" ref="G57" si="11">HEX2DEC(D57)*$A$1</f>
+        <f t="shared" ref="G57" si="19">HEX2DEC(D57)*$A$1</f>
         <v>3.3934000000000002</v>
       </c>
       <c r="H57" s="2">
-        <f t="shared" ref="H57" si="12">HEX2DEC(E57)*$A$1</f>
+        <f t="shared" ref="H57" si="20">HEX2DEC(E57)*$A$1</f>
         <v>3.5720000000000001</v>
       </c>
       <c r="I57" s="2">
-        <f t="shared" ref="I57" si="13">HEX2DEC(F57)*$A$1</f>
+        <f t="shared" ref="I57" si="21">HEX2DEC(F57)*$A$1</f>
         <v>3.1678000000000002</v>
       </c>
       <c r="J57" s="4">
-        <f>AVERAGE(G57:I57)</f>
+        <f t="shared" si="13"/>
         <v>3.3777333333333335</v>
       </c>
       <c r="K57" s="5">
-        <f>VAR(G57:I57)</f>
+        <f t="shared" si="14"/>
         <v>4.1028493333333312E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12">
       <c r="A58">
         <v>20</v>
       </c>
       <c r="B58">
-        <f t="shared" si="7"/>
+        <f t="shared" si="15"/>
         <v>81.231884057970987</v>
       </c>
       <c r="C58" s="6">
@@ -4769,32 +4907,32 @@
         <v>123</v>
       </c>
       <c r="G58" s="2">
-        <f t="shared" ref="G58:G67" si="14">HEX2DEC(D58)*$A$1</f>
+        <f t="shared" ref="G58:G67" si="22">HEX2DEC(D58)*$A$1</f>
         <v>3.1302000000000003</v>
       </c>
       <c r="H58" s="2">
-        <f t="shared" ref="H58:H67" si="15">HEX2DEC(E58)*$A$1</f>
+        <f t="shared" ref="H58:H67" si="23">HEX2DEC(E58)*$A$1</f>
         <v>3.5438000000000001</v>
       </c>
       <c r="I58" s="2">
-        <f t="shared" ref="I58:I67" si="16">HEX2DEC(F58)*$A$1</f>
+        <f t="shared" ref="I58:I67" si="24">HEX2DEC(F58)*$A$1</f>
         <v>3.431</v>
       </c>
       <c r="J58" s="4">
-        <f t="shared" ref="J58:J67" si="17">AVERAGE(G58:I58)</f>
+        <f t="shared" ref="J58:J67" si="25">AVERAGE(G58:I58)</f>
         <v>3.3683333333333336</v>
       </c>
       <c r="K58" s="5">
-        <f t="shared" ref="K58:K67" si="18">VAR(G58:I58)</f>
+        <f t="shared" ref="K58:K67" si="26">VAR(G58:I58)</f>
         <v>4.5711573333333269E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12">
       <c r="A59">
         <v>24</v>
       </c>
       <c r="B59">
-        <f t="shared" si="7"/>
+        <f t="shared" si="15"/>
         <v>98.947826086956496</v>
       </c>
       <c r="C59" s="6">
@@ -4810,32 +4948,32 @@
         <v>134</v>
       </c>
       <c r="G59" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="22"/>
         <v>3.6941999999999999</v>
       </c>
       <c r="H59" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="23"/>
         <v>2.9986000000000002</v>
       </c>
       <c r="I59" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="24"/>
         <v>3.5156000000000001</v>
       </c>
       <c r="J59" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="25"/>
         <v>3.4028000000000005</v>
       </c>
       <c r="K59" s="5">
-        <f t="shared" si="18"/>
+        <f t="shared" si="26"/>
         <v>0.13050771999999994</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12">
       <c r="A60">
         <v>36</v>
       </c>
       <c r="B60">
-        <f t="shared" si="7"/>
+        <f t="shared" si="15"/>
         <v>152.09565217391301</v>
       </c>
       <c r="C60" s="6">
@@ -4851,32 +4989,32 @@
         <v>132</v>
       </c>
       <c r="G60" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="22"/>
         <v>3.4874000000000001</v>
       </c>
       <c r="H60" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="23"/>
         <v>4.0983999999999998</v>
       </c>
       <c r="I60" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="24"/>
         <v>3.5438000000000001</v>
       </c>
       <c r="J60" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="25"/>
         <v>3.7098666666666666</v>
       </c>
       <c r="K60" s="5">
-        <f t="shared" si="18"/>
+        <f t="shared" si="26"/>
         <v>0.11401385333333325</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12">
       <c r="A61">
         <v>47</v>
       </c>
       <c r="B61">
-        <f t="shared" si="7"/>
+        <f t="shared" si="15"/>
         <v>200.81449275362317</v>
       </c>
       <c r="C61" s="6">
@@ -4892,32 +5030,32 @@
         <v>137</v>
       </c>
       <c r="G61" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="22"/>
         <v>3.9104000000000001</v>
       </c>
       <c r="H61" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="23"/>
         <v>4.5026000000000002</v>
       </c>
       <c r="I61" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="24"/>
         <v>4.0890000000000004</v>
       </c>
       <c r="J61" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="25"/>
         <v>4.1673333333333336</v>
       </c>
       <c r="K61" s="5">
-        <f t="shared" si="18"/>
+        <f t="shared" si="26"/>
         <v>9.227729333333333E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12">
       <c r="A62">
         <v>58</v>
       </c>
       <c r="B62">
-        <f t="shared" si="7"/>
+        <f t="shared" si="15"/>
         <v>249.5333333333333</v>
       </c>
       <c r="C62" s="6">
@@ -4933,32 +5071,32 @@
         <v>139</v>
       </c>
       <c r="G62" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="22"/>
         <v>4.2770000000000001</v>
       </c>
       <c r="H62" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="23"/>
         <v>4.9632000000000005</v>
       </c>
       <c r="I62" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="24"/>
         <v>4.6436000000000002</v>
       </c>
       <c r="J62" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="25"/>
         <v>4.6279333333333339</v>
       </c>
       <c r="K62" s="5">
-        <f t="shared" si="18"/>
+        <f t="shared" si="26"/>
         <v>0.11790169333333346</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12">
       <c r="A63">
         <v>70</v>
       </c>
       <c r="B63">
-        <f t="shared" si="7"/>
+        <f t="shared" si="15"/>
         <v>302.68115942028982</v>
       </c>
       <c r="C63" s="6">
@@ -4974,32 +5112,32 @@
         <v>142</v>
       </c>
       <c r="G63" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="22"/>
         <v>5.5084</v>
       </c>
       <c r="H63" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="23"/>
         <v>4.7751999999999999</v>
       </c>
       <c r="I63" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="24"/>
         <v>5.5460000000000003</v>
       </c>
       <c r="J63" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="25"/>
         <v>5.2765333333333331</v>
       </c>
       <c r="K63" s="5">
-        <f t="shared" si="18"/>
+        <f t="shared" si="26"/>
         <v>0.18885477333333345</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12">
       <c r="A64">
         <v>81</v>
       </c>
       <c r="B64">
-        <f t="shared" si="7"/>
+        <f t="shared" si="15"/>
         <v>351.4</v>
       </c>
       <c r="C64" s="6">
@@ -5015,32 +5153,32 @@
         <v>99</v>
       </c>
       <c r="G64" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="22"/>
         <v>5.4332000000000003</v>
       </c>
       <c r="H64" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="23"/>
         <v>6.2040000000000006</v>
       </c>
       <c r="I64" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="24"/>
         <v>5.875</v>
       </c>
       <c r="J64" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="25"/>
         <v>5.8373999999999997</v>
       </c>
       <c r="K64" s="5">
-        <f t="shared" si="18"/>
+        <f t="shared" si="26"/>
         <v>0.14959348000000014</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11">
       <c r="A65">
         <v>92</v>
       </c>
       <c r="B65">
-        <f t="shared" si="7"/>
+        <f t="shared" si="15"/>
         <v>400.11884057971014</v>
       </c>
       <c r="C65" s="6">
@@ -5056,32 +5194,32 @@
         <v>146</v>
       </c>
       <c r="G65" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="22"/>
         <v>6.8338000000000001</v>
       </c>
       <c r="H65" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="23"/>
         <v>6.5330000000000004</v>
       </c>
       <c r="I65" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="24"/>
         <v>6.1194000000000006</v>
       </c>
       <c r="J65" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="25"/>
         <v>6.495400000000001</v>
       </c>
       <c r="K65" s="5">
-        <f t="shared" si="18"/>
+        <f t="shared" si="26"/>
         <v>0.12865215999999982</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11">
       <c r="A66">
         <v>103</v>
       </c>
       <c r="B66">
-        <f t="shared" si="7"/>
+        <f t="shared" si="15"/>
         <v>448.83768115942024</v>
       </c>
       <c r="C66" s="6">
@@ -5097,32 +5235,32 @@
         <v>147</v>
       </c>
       <c r="G66" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="22"/>
         <v>7.3790000000000004</v>
       </c>
       <c r="H66" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="23"/>
         <v>6.6928000000000001</v>
       </c>
       <c r="I66" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="24"/>
         <v>7.3790000000000004</v>
       </c>
       <c r="J66" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="25"/>
         <v>7.150266666666667</v>
       </c>
       <c r="K66" s="5">
-        <f t="shared" si="18"/>
+        <f t="shared" si="26"/>
         <v>0.1569568133333335</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11">
       <c r="A67">
         <v>113</v>
       </c>
       <c r="B67">
-        <f t="shared" si="7"/>
+        <f t="shared" si="15"/>
         <v>493.12753623188399</v>
       </c>
       <c r="C67" s="6">
@@ -5138,27 +5276,27 @@
         <v>151</v>
       </c>
       <c r="G67" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="22"/>
         <v>7.0030000000000001</v>
       </c>
       <c r="H67" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="23"/>
         <v>7.99</v>
       </c>
       <c r="I67" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="24"/>
         <v>7.3601999999999999</v>
       </c>
       <c r="J67" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="25"/>
         <v>7.4510666666666667</v>
       </c>
       <c r="K67" s="5">
-        <f t="shared" si="18"/>
+        <f t="shared" si="26"/>
         <v>0.24973481333333339</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11">
       <c r="C68" s="6"/>
       <c r="F68" s="2"/>
       <c r="G68" s="2"/>
@@ -5167,7 +5305,7 @@
       <c r="J68" s="4"/>
       <c r="K68" s="5"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11">
       <c r="C69" s="6"/>
       <c r="F69" s="2"/>
       <c r="G69" s="2"/>
@@ -5176,7 +5314,7 @@
       <c r="J69" s="4"/>
       <c r="K69" s="5"/>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11">
       <c r="C70" s="6"/>
       <c r="F70" s="2"/>
       <c r="G70" s="2"/>
@@ -5185,38 +5323,43 @@
       <c r="J70" s="4"/>
       <c r="K70" s="5"/>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11">
       <c r="C71" s="6"/>
       <c r="F71" s="2"/>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11">
       <c r="C72" s="6"/>
       <c r="F72" s="2"/>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11">
       <c r="C73" s="6"/>
       <c r="F73" s="2"/>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11">
       <c r="C74" s="6"/>
       <c r="F74" s="2"/>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11">
       <c r="C75" s="6"/>
       <c r="F75" s="2"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11">
       <c r="C76" s="6"/>
       <c r="F76" s="2"/>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11">
       <c r="C77" s="6"/>
       <c r="F77" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup orientation="portrait"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -5226,9 +5369,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -5238,8 +5386,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>